<commit_message>
Large scale distributed deep networks
</commit_message>
<xml_diff>
--- a/Working Progress Timetable/Time sheet 2.xlsx
+++ b/Working Progress Timetable/Time sheet 2.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="27-5-2018 to 3-6-2018" sheetId="1" r:id="rId1"/>
+    <sheet name="5-6-2018 to 10-6-2018" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Report Duration</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>Start Reading Deep Learning in Neural Networks: An Overview (15 page)</t>
+  </si>
+  <si>
+    <t>Reading  Large Scale Distributed Deep Networks</t>
+  </si>
+  <si>
+    <t>Tensorflow  Hands on mini batch stochastic gradeint descent (SGD)</t>
   </si>
 </sst>
 </file>
@@ -281,6 +287,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -294,18 +312,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -615,7 +621,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:F17"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -630,10 +636,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33.6" customHeight="1" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="19"/>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
@@ -656,28 +662,28 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="33.6" customHeight="1">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:11" ht="24.6" customHeight="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="17"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
       <c r="I4" s="12" t="s">
         <v>7</v>
       </c>
@@ -695,11 +701,11 @@
       <c r="C5" s="8">
         <v>6</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="14">
         <v>43196</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
       <c r="A6" s="6">
@@ -711,11 +717,11 @@
       <c r="C6" s="8">
         <v>2</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="14">
         <v>43226</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1">
       <c r="A7" s="9">
@@ -727,11 +733,11 @@
       <c r="C7" s="9">
         <v>7</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="15">
         <v>43257</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
       <c r="A8" s="9">
@@ -741,13 +747,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="9">
-        <v>2</v>
-      </c>
-      <c r="D8" s="20">
+        <v>4</v>
+      </c>
+      <c r="D8" s="15">
         <v>43257</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
       <c r="A9" s="9">
@@ -759,132 +765,148 @@
       <c r="C9" s="9">
         <v>7</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="15">
         <v>43287</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
+      <c r="A10" s="8">
+        <v>6</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8">
+        <v>5</v>
+      </c>
+      <c r="D10" s="14">
+        <v>43318</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:11" ht="14.4">
-      <c r="A11" s="6"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
+      <c r="A11" s="6">
+        <v>7</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2</v>
+      </c>
+      <c r="D11" s="14">
+        <v>43318</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:11" ht="14.4">
       <c r="A12" s="9"/>
       <c r="B12" s="11"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:11" ht="14.4">
       <c r="A13" s="6"/>
       <c r="B13" s="11"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:11" ht="14.4">
       <c r="A14" s="9"/>
       <c r="B14" s="11"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:11" ht="14.4">
       <c r="A15" s="8"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:11" ht="14.4">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" ht="14.4">
       <c r="A17" s="9"/>
       <c r="B17" s="7"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" ht="14.4">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" ht="14.4">
       <c r="A19" s="9"/>
       <c r="B19" s="7"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:6" ht="14.4">
       <c r="A20" s="8"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" ht="14.4">
       <c r="A21" s="9"/>
       <c r="B21" s="7"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="D4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Weekly Progress - week 2
</commit_message>
<xml_diff>
--- a/Working Progress Timetable/Time sheet 2.xlsx
+++ b/Working Progress Timetable/Time sheet 2.xlsx
@@ -287,18 +287,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -312,6 +300,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,7 +621,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D13" sqref="D13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -636,10 +636,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33.6" customHeight="1" thickBot="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="15"/>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
@@ -662,28 +662,28 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="33.6" customHeight="1">
-      <c r="A3" s="20"/>
-      <c r="B3" s="21" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:11" ht="24.6" customHeight="1">
-      <c r="A4" s="20"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
       <c r="I4" s="12" t="s">
         <v>7</v>
       </c>
@@ -701,11 +701,11 @@
       <c r="C5" s="8">
         <v>6</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="19">
         <v>43196</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
       <c r="A6" s="6">
@@ -717,11 +717,11 @@
       <c r="C6" s="8">
         <v>2</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="19">
         <v>43226</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1">
       <c r="A7" s="9">
@@ -733,11 +733,11 @@
       <c r="C7" s="9">
         <v>7</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="20">
         <v>43257</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
       <c r="A8" s="9">
@@ -749,11 +749,11 @@
       <c r="C8" s="9">
         <v>4</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="20">
         <v>43257</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
       <c r="A9" s="9">
@@ -765,11 +765,11 @@
       <c r="C9" s="9">
         <v>7</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="20">
         <v>43287</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
       <c r="A10" s="8">
@@ -781,11 +781,11 @@
       <c r="C10" s="8">
         <v>5</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="19">
         <v>43318</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:11" ht="14.4">
       <c r="A11" s="6">
@@ -797,116 +797,116 @@
       <c r="C11" s="8">
         <v>2</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="19">
         <v>43318</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:11" ht="14.4">
       <c r="A12" s="9"/>
       <c r="B12" s="11"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:11" ht="14.4">
       <c r="A13" s="6"/>
       <c r="B13" s="11"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:11" ht="14.4">
       <c r="A14" s="9"/>
       <c r="B14" s="11"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:11" ht="14.4">
       <c r="A15" s="8"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
     </row>
     <row r="16" spans="1:11" ht="14.4">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="14.4">
       <c r="A17" s="9"/>
       <c r="B17" s="7"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" ht="14.4">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:6" ht="14.4">
       <c r="A19" s="9"/>
       <c r="B19" s="7"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
     </row>
     <row r="20" spans="1:6" ht="14.4">
       <c r="A20" s="8"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:6" ht="14.4">
       <c r="A21" s="9"/>
       <c r="B21" s="7"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="D4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>